<commit_message>
fixed the left and right problem
</commit_message>
<xml_diff>
--- a/Lab02/Code/SensorCalibration/SensorData.xlsx
+++ b/Lab02/Code/SensorCalibration/SensorData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adairdg\Documents\Classes\ECE-425-Mobile-Robotics\Lab02\Code\SensorCalibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EA86C4-4655-4FF3-B362-704D42A6408C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A6B93-079F-40AE-9B31-B2765A916B93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7B5C36B3-28DB-4FDE-A3F1-AA54B0BA1D69}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Acutal Inches</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Inches = 285714/(R+2257) - 102</t>
+  </si>
+  <si>
+    <t>Inches = 568181 / (R+11136) - 50</t>
+  </si>
+  <si>
+    <t>Inches = 479616 / (R + 9520) - 50</t>
   </si>
 </sst>
 </file>
@@ -2323,6 +2329,994 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1569553805774279E-2"/>
+                  <c:y val="-0.14985272674249053"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$142:$A$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1535</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1665</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2220</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2370</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2535</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2670</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3620</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2950</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$142:$B$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.9607843137254902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9230769230769232E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8867924528301886E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8518518518518517E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8181818181818181E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7857142857142856E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7543859649122806E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7241379310344827E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6949152542372881E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6393442622950821E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6129032258064516E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5873015873015872E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5625E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5384615384615385E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5151515151515152E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4925373134328358E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4705882352941176E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4492753623188406E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4285714285714285E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-37C0-4E25-B394-F093F26CD058}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="550860984"/>
+        <c:axId val="550860328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="550860984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="550860328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="550860328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="550860984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.3167979002624668E-2"/>
+                  <c:y val="-0.72320902595508896"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$165:$A$184</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>765</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1670</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1770</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1910</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2155</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2385</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2410</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2620</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2775</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$165:$B$184</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.9607843137254902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9230769230769232E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8867924528301886E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8518518518518517E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8181818181818181E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7857142857142856E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7543859649122806E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7241379310344827E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6949152542372881E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6393442622950821E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6129032258064516E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5873015873015872E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5625E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5384615384615385E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5151515151515152E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4925373134328358E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4705882352941176E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4492753623188406E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4285714285714285E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FB8D-435B-AC19-C9DC932ADB23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="441244640"/>
+        <c:axId val="441245624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="441244640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441245624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="441245624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441244640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2483,6 +3477,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4032,6 +5106,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4688,6 +6794,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{801EA181-7EE9-45E8-8747-8B7E85EF509E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA854EF3-F850-4ABC-BC47-017AD69B2128}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4996,7 +7174,7 @@
   <dimension ref="A1:M184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6023,13 +8201,23 @@
       <c r="B27" s="4">
         <v>390</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="4">
+        <f>100*ABS(C27-A27)/A27</f>
+        <v>100</v>
+      </c>
       <c r="E27" s="4">
         <v>350</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="4"/>
+      <c r="F27" s="3">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4">
+        <f>100*ABS(F27-A27)/A27</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
@@ -6038,13 +8226,23 @@
       <c r="B28" s="4">
         <v>450</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" ref="D28:D46" si="4">100*ABS(C28-A28)/A28</f>
+        <v>0</v>
+      </c>
       <c r="E28" s="4">
         <v>430</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
+      <c r="F28" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" ref="G28:G46" si="5">100*ABS(F28-A28)/A28</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
@@ -6053,13 +8251,23 @@
       <c r="B29" s="4">
         <v>555</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E29" s="4">
         <v>490</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
+      <c r="F29" s="3">
+        <v>3</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
@@ -6068,13 +8276,23 @@
       <c r="B30" s="4">
         <v>645</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
+      <c r="C30" s="3">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E30" s="4">
         <v>580</v>
       </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="4"/>
+      <c r="F30" s="3">
+        <v>4</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
@@ -6083,13 +8301,23 @@
       <c r="B31" s="4">
         <v>790</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
+      <c r="C31" s="3">
+        <v>5</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E31" s="4">
         <v>765</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="4"/>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
@@ -6098,13 +8326,23 @@
       <c r="B32" s="4">
         <v>940</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
+      <c r="C32" s="3">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E32" s="4">
         <v>910</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="4"/>
+      <c r="F32" s="3">
+        <v>5</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="5"/>
+        <v>16.666666666666668</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
@@ -6113,13 +8351,23 @@
       <c r="B33" s="4">
         <v>1090</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
+      <c r="C33" s="3">
+        <v>7</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E33" s="4">
         <v>1050</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="4"/>
+      <c r="F33" s="3">
+        <v>6</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="5"/>
+        <v>14.285714285714286</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -6128,13 +8376,23 @@
       <c r="B34" s="4">
         <v>1215</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
+      <c r="C34" s="3">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E34" s="4">
         <v>1235</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="4"/>
+      <c r="F34" s="3">
+        <v>7</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
@@ -6143,13 +8401,23 @@
       <c r="B35" s="4">
         <v>1380</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
+      <c r="C35" s="3">
+        <v>9</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E35" s="4">
         <v>1370</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="4"/>
+      <c r="F35" s="3">
+        <v>7</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="5"/>
+        <v>22.222222222222221</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
@@ -6158,13 +8426,23 @@
       <c r="B36" s="4">
         <v>1535</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
+      <c r="C36" s="3">
+        <v>10</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E36" s="4">
         <v>1450</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="4"/>
+      <c r="F36" s="3">
+        <v>8</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
@@ -6173,13 +8451,23 @@
       <c r="B37" s="4">
         <v>1665</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
+      <c r="C37" s="3">
+        <v>11</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E37" s="4">
         <v>1670</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="4"/>
+      <c r="F37" s="3">
+        <v>8</v>
+      </c>
+      <c r="G37" s="4">
+        <f t="shared" si="5"/>
+        <v>27.272727272727273</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
@@ -6188,13 +8476,23 @@
       <c r="B38" s="4">
         <v>1810</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
+      <c r="C38" s="3">
+        <v>12</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E38" s="4">
         <v>1620</v>
       </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="4"/>
+      <c r="F38" s="3">
+        <v>9</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
@@ -6203,13 +8501,23 @@
       <c r="B39" s="4">
         <v>1975</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="3">
+        <v>13</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="E39" s="4">
         <v>1770</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="4"/>
+      <c r="F39" s="3">
+        <v>10</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" si="5"/>
+        <v>23.076923076923077</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
@@ -6218,13 +8526,23 @@
       <c r="B40" s="4">
         <v>2095</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
+      <c r="C40" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="4"/>
+        <v>3.5714285714285716</v>
+      </c>
       <c r="E40" s="4">
         <v>1910</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="4"/>
+      <c r="F40" s="3">
+        <v>10</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="5"/>
+        <v>28.571428571428573</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
@@ -6233,13 +8551,23 @@
       <c r="B41" s="4">
         <v>2220</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="3">
+        <v>16</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="4"/>
+        <v>6.666666666666667</v>
+      </c>
       <c r="E41" s="4">
         <v>2155</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="3">
+        <v>12</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
@@ -6248,13 +8576,23 @@
       <c r="B42" s="4">
         <v>2370</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="3">
+        <v>17</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="4"/>
+        <v>6.25</v>
+      </c>
       <c r="E42" s="4">
         <v>2385</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="4"/>
+      <c r="F42" s="3">
+        <v>13</v>
+      </c>
+      <c r="G42" s="4">
+        <f t="shared" si="5"/>
+        <v>18.75</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
@@ -6263,13 +8601,23 @@
       <c r="B43" s="4">
         <v>2535</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="3">
+        <v>19</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="4"/>
+        <v>11.764705882352942</v>
+      </c>
       <c r="E43" s="4">
         <v>2410</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="4"/>
+      <c r="F43" s="3">
+        <v>16</v>
+      </c>
+      <c r="G43" s="4">
+        <f t="shared" si="5"/>
+        <v>5.882352941176471</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
@@ -6278,13 +8626,23 @@
       <c r="B44" s="4">
         <v>2670</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="4"/>
+      <c r="C44" s="3">
+        <v>20</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="4"/>
+        <v>11.111111111111111</v>
+      </c>
       <c r="E44" s="4">
         <v>2500</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="4"/>
+      <c r="F44" s="3">
+        <v>17</v>
+      </c>
+      <c r="G44" s="4">
+        <f t="shared" si="5"/>
+        <v>5.5555555555555554</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
@@ -6293,13 +8651,23 @@
       <c r="B45" s="4">
         <v>3620</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
+      <c r="C45" s="3">
+        <v>22</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="4"/>
+        <v>15.789473684210526</v>
+      </c>
       <c r="E45" s="4">
         <v>2620</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="4"/>
+      <c r="F45" s="3">
+        <v>18</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" si="5"/>
+        <v>5.2631578947368425</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
@@ -6308,20 +8676,30 @@
       <c r="B46" s="4">
         <v>2950</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="4"/>
+      <c r="C46" s="3">
+        <v>23</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
       <c r="E46" s="4">
         <v>2775</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="4"/>
+      <c r="F46" s="3">
+        <v>18</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>530</v>
       </c>
       <c r="B50">
-        <f>1/(A3+1)</f>
+        <f t="shared" ref="B50:B69" si="6">1/(A3+1)</f>
         <v>0.5</v>
       </c>
     </row>
@@ -6330,7 +8708,7 @@
         <v>370</v>
       </c>
       <c r="B51">
-        <f>1/(A4+1)</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -6339,7 +8717,7 @@
         <v>270</v>
       </c>
       <c r="B52">
-        <f>1/(A5+1)</f>
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
     </row>
@@ -6348,7 +8726,7 @@
         <v>210</v>
       </c>
       <c r="B53">
-        <f>1/(A6+1)</f>
+        <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
     </row>
@@ -6357,7 +8735,7 @@
         <v>170</v>
       </c>
       <c r="B54">
-        <f>1/(A7+1)</f>
+        <f t="shared" si="6"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -6366,7 +8744,7 @@
         <v>140</v>
       </c>
       <c r="B55">
-        <f>1/(A8+1)</f>
+        <f t="shared" si="6"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -6375,7 +8753,7 @@
         <v>125</v>
       </c>
       <c r="B56">
-        <f>1/(A9+1)</f>
+        <f t="shared" si="6"/>
         <v>0.125</v>
       </c>
     </row>
@@ -6384,7 +8762,7 @@
         <v>110</v>
       </c>
       <c r="B57">
-        <f>1/(A10+1)</f>
+        <f t="shared" si="6"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -6393,7 +8771,7 @@
         <v>95</v>
       </c>
       <c r="B58">
-        <f>1/(A11+1)</f>
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6402,7 +8780,7 @@
         <v>80</v>
       </c>
       <c r="B59">
-        <f>1/(A12+1)</f>
+        <f t="shared" si="6"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
@@ -6411,7 +8789,7 @@
         <v>75</v>
       </c>
       <c r="B60">
-        <f>1/(A13+1)</f>
+        <f t="shared" si="6"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -6420,7 +8798,7 @@
         <v>70</v>
       </c>
       <c r="B61">
-        <f>1/(A14+1)</f>
+        <f t="shared" si="6"/>
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
@@ -6429,7 +8807,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <f>1/(A15+1)</f>
+        <f t="shared" si="6"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -6438,7 +8816,7 @@
         <v>50</v>
       </c>
       <c r="B63">
-        <f>1/(A16+1)</f>
+        <f t="shared" si="6"/>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
@@ -6447,7 +8825,7 @@
         <v>50</v>
       </c>
       <c r="B64">
-        <f>1/(A17+1)</f>
+        <f t="shared" si="6"/>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -6456,7 +8834,7 @@
         <v>50</v>
       </c>
       <c r="B65">
-        <f>1/(A18+1)</f>
+        <f t="shared" si="6"/>
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
@@ -6465,7 +8843,7 @@
         <v>50</v>
       </c>
       <c r="B66">
-        <f>1/(A19+1)</f>
+        <f t="shared" si="6"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
@@ -6474,7 +8852,7 @@
         <v>45</v>
       </c>
       <c r="B67">
-        <f>1/(A20+1)</f>
+        <f t="shared" si="6"/>
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
@@ -6483,7 +8861,7 @@
         <v>40</v>
       </c>
       <c r="B68">
-        <f>1/(A21+1)</f>
+        <f t="shared" si="6"/>
         <v>0.05</v>
       </c>
       <c r="C68" t="s">
@@ -6495,7 +8873,7 @@
         <v>45</v>
       </c>
       <c r="B69">
-        <f>1/(A22+1)</f>
+        <f t="shared" si="6"/>
         <v>4.7619047619047616E-2</v>
       </c>
     </row>
@@ -6518,7 +8896,7 @@
         <v>345</v>
       </c>
       <c r="B74">
-        <f t="shared" ref="B74:B92" si="4">1/(A4+1)</f>
+        <f t="shared" ref="B74:B92" si="7">1/(A4+1)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -6527,7 +8905,7 @@
         <v>240</v>
       </c>
       <c r="B75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
     </row>
@@ -6536,7 +8914,7 @@
         <v>190</v>
       </c>
       <c r="B76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
     </row>
@@ -6545,7 +8923,7 @@
         <v>155</v>
       </c>
       <c r="B77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -6554,7 +8932,7 @@
         <v>135</v>
       </c>
       <c r="B78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -6563,7 +8941,7 @@
         <v>110</v>
       </c>
       <c r="B79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.125</v>
       </c>
     </row>
@@ -6572,7 +8950,7 @@
         <v>95</v>
       </c>
       <c r="B80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -6581,7 +8959,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6590,7 +8968,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
@@ -6599,7 +8977,7 @@
         <v>70</v>
       </c>
       <c r="B83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -6608,7 +8986,7 @@
         <v>65</v>
       </c>
       <c r="B84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
@@ -6617,7 +8995,7 @@
         <v>50</v>
       </c>
       <c r="B85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -6626,7 +9004,7 @@
         <v>60</v>
       </c>
       <c r="B86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
@@ -6635,7 +9013,7 @@
         <v>45</v>
       </c>
       <c r="B87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -6644,7 +9022,7 @@
         <v>45</v>
       </c>
       <c r="B88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
@@ -6653,7 +9031,7 @@
         <v>40</v>
       </c>
       <c r="B89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
@@ -6662,7 +9040,7 @@
         <v>40</v>
       </c>
       <c r="B90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="C90" t="s">
@@ -6674,7 +9052,7 @@
         <v>45</v>
       </c>
       <c r="B91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.05</v>
       </c>
     </row>
@@ -6683,7 +9061,7 @@
         <v>50</v>
       </c>
       <c r="B92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4.7619047619047616E-2</v>
       </c>
     </row>
@@ -6706,7 +9084,7 @@
         <v>655</v>
       </c>
       <c r="B97">
-        <f t="shared" ref="B97:B115" si="5">1/(A4+105)</f>
+        <f t="shared" ref="B97:B115" si="8">1/(A4+105)</f>
         <v>9.3457943925233638E-3</v>
       </c>
     </row>
@@ -6715,7 +9093,7 @@
         <v>600</v>
       </c>
       <c r="B98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.2592592592592587E-3</v>
       </c>
     </row>
@@ -6724,7 +9102,7 @@
         <v>490</v>
       </c>
       <c r="B99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.1743119266055051E-3</v>
       </c>
     </row>
@@ -6733,7 +9111,7 @@
         <v>405</v>
       </c>
       <c r="B100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.0909090909090905E-3</v>
       </c>
     </row>
@@ -6742,7 +9120,7 @@
         <v>350</v>
       </c>
       <c r="B101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9.0090090090090089E-3</v>
       </c>
     </row>
@@ -6751,7 +9129,7 @@
         <v>305</v>
       </c>
       <c r="B102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.9285714285714281E-3</v>
       </c>
     </row>
@@ -6760,7 +9138,7 @@
         <v>275</v>
       </c>
       <c r="B103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.8495575221238937E-3</v>
       </c>
     </row>
@@ -6769,7 +9147,7 @@
         <v>250</v>
       </c>
       <c r="B104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.771929824561403E-3</v>
       </c>
     </row>
@@ -6778,7 +9156,7 @@
         <v>235</v>
       </c>
       <c r="B105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.6956521739130436E-3</v>
       </c>
     </row>
@@ -6787,7 +9165,7 @@
         <v>215</v>
       </c>
       <c r="B106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.6206896551724137E-3</v>
       </c>
     </row>
@@ -6796,7 +9174,7 @@
         <v>205</v>
       </c>
       <c r="B107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.5470085470085479E-3</v>
       </c>
     </row>
@@ -6805,7 +9183,7 @@
         <v>200</v>
       </c>
       <c r="B108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.4745762711864406E-3</v>
       </c>
     </row>
@@ -6814,7 +9192,7 @@
         <v>190</v>
       </c>
       <c r="B109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.4033613445378148E-3</v>
       </c>
     </row>
@@ -6823,7 +9201,7 @@
         <v>185</v>
       </c>
       <c r="B110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
@@ -6832,7 +9210,7 @@
         <v>180</v>
       </c>
       <c r="B111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.2644628099173556E-3</v>
       </c>
     </row>
@@ -6841,7 +9219,7 @@
         <v>175</v>
       </c>
       <c r="B112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.1967213114754103E-3</v>
       </c>
     </row>
@@ -6850,7 +9228,7 @@
         <v>180</v>
       </c>
       <c r="B113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.130081300813009E-3</v>
       </c>
       <c r="C113" t="s">
@@ -6862,7 +9240,7 @@
         <v>175</v>
       </c>
       <c r="B114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.0645161290322578E-3</v>
       </c>
     </row>
@@ -6871,7 +9249,7 @@
         <v>180</v>
       </c>
       <c r="B115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
@@ -6889,7 +9267,7 @@
         <v>667</v>
       </c>
       <c r="B120">
-        <f t="shared" ref="B120:B138" si="6">1/(A4+75)</f>
+        <f t="shared" ref="B120:B138" si="9">1/(A4+75)</f>
         <v>1.2987012987012988E-2</v>
       </c>
     </row>
@@ -6898,7 +9276,7 @@
         <v>625</v>
       </c>
       <c r="B121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.282051282051282E-2</v>
       </c>
     </row>
@@ -6907,7 +9285,7 @@
         <v>500</v>
       </c>
       <c r="B122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2658227848101266E-2</v>
       </c>
     </row>
@@ -6916,7 +9294,7 @@
         <v>415</v>
       </c>
       <c r="B123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
@@ -6925,7 +9303,7 @@
         <v>340</v>
       </c>
       <c r="B124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2345679012345678E-2</v>
       </c>
     </row>
@@ -6934,7 +9312,7 @@
         <v>305</v>
       </c>
       <c r="B125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2195121951219513E-2</v>
       </c>
     </row>
@@ -6943,7 +9321,7 @@
         <v>275</v>
       </c>
       <c r="B126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2048192771084338E-2</v>
       </c>
     </row>
@@ -6952,7 +9330,7 @@
         <v>245</v>
       </c>
       <c r="B127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1904761904761904E-2</v>
       </c>
     </row>
@@ -6961,7 +9339,7 @@
         <v>225</v>
       </c>
       <c r="B128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1764705882352941E-2</v>
       </c>
     </row>
@@ -6970,7 +9348,7 @@
         <v>205</v>
       </c>
       <c r="B129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
@@ -6979,7 +9357,7 @@
         <v>190</v>
       </c>
       <c r="B130">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1494252873563218E-2</v>
       </c>
     </row>
@@ -6988,7 +9366,7 @@
         <v>180</v>
       </c>
       <c r="B131">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1363636363636364E-2</v>
       </c>
     </row>
@@ -6997,7 +9375,7 @@
         <v>170</v>
       </c>
       <c r="B132">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1235955056179775E-2</v>
       </c>
     </row>
@@ -7006,7 +9384,7 @@
         <v>160</v>
       </c>
       <c r="B133">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
@@ -7015,7 +9393,7 @@
         <v>150</v>
       </c>
       <c r="B134">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.098901098901099E-2</v>
       </c>
     </row>
@@ -7024,7 +9402,7 @@
         <v>145</v>
       </c>
       <c r="B135">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.0869565217391304E-2</v>
       </c>
       <c r="C135" t="s">
@@ -7036,7 +9414,7 @@
         <v>140</v>
       </c>
       <c r="B136">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.0752688172043012E-2</v>
       </c>
     </row>
@@ -7045,7 +9423,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.0638297872340425E-2</v>
       </c>
     </row>
@@ -7054,7 +9432,7 @@
         <v>130</v>
       </c>
       <c r="B138">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.0526315789473684E-2</v>
       </c>
     </row>
@@ -7063,8 +9441,8 @@
         <v>390</v>
       </c>
       <c r="B142">
-        <f>1/(A142+1)</f>
-        <v>2.5575447570332483E-3</v>
+        <f>1/(A3+50)</f>
+        <v>1.9607843137254902E-2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -7072,8 +9450,8 @@
         <v>450</v>
       </c>
       <c r="B143">
-        <f t="shared" ref="B143:B161" si="7">1/(A143+1)</f>
-        <v>2.2172949002217295E-3</v>
+        <f t="shared" ref="B143:B161" si="10">1/(A4+50)</f>
+        <v>1.9230769230769232E-2</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -7081,152 +9459,155 @@
         <v>555</v>
       </c>
       <c r="B144">
-        <f t="shared" si="7"/>
-        <v>1.7985611510791368E-3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.8867924528301886E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>645</v>
       </c>
       <c r="B145">
-        <f t="shared" si="7"/>
-        <v>1.5479876160990713E-3</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.8518518518518517E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>790</v>
       </c>
       <c r="B146">
-        <f t="shared" si="7"/>
-        <v>1.2642225031605564E-3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.8181818181818181E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>940</v>
       </c>
       <c r="B147">
-        <f t="shared" si="7"/>
-        <v>1.0626992561105207E-3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.7857142857142856E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
         <v>1090</v>
       </c>
       <c r="B148">
-        <f t="shared" si="7"/>
-        <v>9.1659028414298811E-4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.7543859649122806E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>1215</v>
       </c>
       <c r="B149">
-        <f t="shared" si="7"/>
-        <v>8.2236842105263153E-4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.7241379310344827E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>1380</v>
       </c>
       <c r="B150">
-        <f t="shared" si="7"/>
-        <v>7.2411296162201298E-4</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.6949152542372881E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>1535</v>
       </c>
       <c r="B151">
-        <f t="shared" si="7"/>
-        <v>6.5104166666666663E-4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
         <v>1665</v>
       </c>
       <c r="B152">
-        <f t="shared" si="7"/>
-        <v>6.0024009603841532E-4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.6393442622950821E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="4">
         <v>1810</v>
       </c>
       <c r="B153">
-        <f t="shared" si="7"/>
-        <v>5.5218111540585317E-4</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.6129032258064516E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="4">
         <v>1975</v>
       </c>
       <c r="B154">
-        <f t="shared" si="7"/>
-        <v>5.0607287449392713E-4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.5873015873015872E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="4">
         <v>2095</v>
       </c>
       <c r="B155">
-        <f t="shared" si="7"/>
-        <v>4.7709923664122136E-4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="4">
         <v>2220</v>
       </c>
       <c r="B156">
-        <f t="shared" si="7"/>
-        <v>4.5024763619990995E-4</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="4">
         <v>2370</v>
       </c>
       <c r="B157">
-        <f t="shared" si="7"/>
-        <v>4.2176296921130323E-4</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="4">
         <v>2535</v>
       </c>
       <c r="B158">
-        <f t="shared" si="7"/>
-        <v>3.9432176656151418E-4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.4925373134328358E-2</v>
+      </c>
+      <c r="C158" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="4">
         <v>2670</v>
       </c>
       <c r="B159">
-        <f t="shared" si="7"/>
-        <v>3.7439161362785476E-4</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.4705882352941176E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="4">
         <v>3620</v>
       </c>
       <c r="B160">
-        <f t="shared" si="7"/>
-        <v>2.7616680475006904E-4</v>
+        <f t="shared" si="10"/>
+        <v>1.4492753623188406E-2</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -7234,8 +9615,8 @@
         <v>2950</v>
       </c>
       <c r="B161">
-        <f t="shared" si="7"/>
-        <v>3.3886818027787193E-4</v>
+        <f t="shared" si="10"/>
+        <v>1.4285714285714285E-2</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -7243,8 +9624,8 @@
         <v>350</v>
       </c>
       <c r="B165">
-        <f>1/(A165+1)</f>
-        <v>2.8490028490028491E-3</v>
+        <f>1/(A3+50)</f>
+        <v>1.9607843137254902E-2</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -7252,8 +9633,8 @@
         <v>430</v>
       </c>
       <c r="B166">
-        <f t="shared" ref="B166:B184" si="8">1/(A166+1)</f>
-        <v>2.3201856148491878E-3</v>
+        <f t="shared" ref="B166:B184" si="11">1/(A4+50)</f>
+        <v>1.9230769230769232E-2</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -7261,8 +9642,8 @@
         <v>490</v>
       </c>
       <c r="B167">
-        <f t="shared" si="8"/>
-        <v>2.0366598778004071E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.8867924528301886E-2</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -7270,8 +9651,8 @@
         <v>580</v>
       </c>
       <c r="B168">
-        <f t="shared" si="8"/>
-        <v>1.7211703958691911E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.8518518518518517E-2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -7279,8 +9660,8 @@
         <v>765</v>
       </c>
       <c r="B169">
-        <f t="shared" si="8"/>
-        <v>1.3054830287206266E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.8181818181818181E-2</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
@@ -7288,8 +9669,8 @@
         <v>910</v>
       </c>
       <c r="B170">
-        <f t="shared" si="8"/>
-        <v>1.0976948408342481E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.7857142857142856E-2</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -7297,8 +9678,8 @@
         <v>1050</v>
       </c>
       <c r="B171">
-        <f t="shared" si="8"/>
-        <v>9.5147478591817321E-4</v>
+        <f t="shared" si="11"/>
+        <v>1.7543859649122806E-2</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -7306,8 +9687,8 @@
         <v>1235</v>
       </c>
       <c r="B172">
-        <f t="shared" si="8"/>
-        <v>8.090614886731392E-4</v>
+        <f t="shared" si="11"/>
+        <v>1.7241379310344827E-2</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -7315,8 +9696,8 @@
         <v>1370</v>
       </c>
       <c r="B173">
-        <f t="shared" si="8"/>
-        <v>7.2939460247994166E-4</v>
+        <f t="shared" si="11"/>
+        <v>1.6949152542372881E-2</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -7324,8 +9705,8 @@
         <v>1450</v>
       </c>
       <c r="B174">
-        <f t="shared" si="8"/>
-        <v>6.8917987594762232E-4</v>
+        <f t="shared" si="11"/>
+        <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -7333,8 +9714,8 @@
         <v>1670</v>
       </c>
       <c r="B175">
-        <f t="shared" si="8"/>
-        <v>5.9844404548174744E-4</v>
+        <f t="shared" si="11"/>
+        <v>1.6393442622950821E-2</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -7342,80 +9723,83 @@
         <v>1620</v>
       </c>
       <c r="B176">
-        <f t="shared" si="8"/>
-        <v>6.1690314620604567E-4</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.6129032258064516E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="4">
         <v>1770</v>
       </c>
       <c r="B177">
-        <f t="shared" si="8"/>
-        <v>5.6465273856578201E-4</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.5873015873015872E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="4">
         <v>1910</v>
       </c>
       <c r="B178">
-        <f t="shared" si="8"/>
-        <v>5.2328623757195189E-4</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="4">
         <v>2155</v>
       </c>
       <c r="B179">
-        <f t="shared" si="8"/>
-        <v>4.6382189239332097E-4</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="4">
         <v>2385</v>
       </c>
       <c r="B180">
-        <f t="shared" si="8"/>
-        <v>4.1911148365465214E-4</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="4">
         <v>2410</v>
       </c>
       <c r="B181">
-        <f t="shared" si="8"/>
-        <v>4.1476565740356696E-4</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.4925373134328358E-2</v>
+      </c>
+      <c r="C181" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="4">
         <v>2500</v>
       </c>
       <c r="B182">
-        <f t="shared" si="8"/>
-        <v>3.9984006397441024E-4</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.4705882352941176E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="4">
         <v>2620</v>
       </c>
       <c r="B183">
-        <f t="shared" si="8"/>
-        <v>3.8153376573826786E-4</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>1.4492753623188406E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="4">
         <v>2775</v>
       </c>
       <c r="B184">
-        <f t="shared" si="8"/>
-        <v>3.6023054755043225E-4</v>
+        <f t="shared" si="11"/>
+        <v>1.4285714285714285E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>